<commit_message>
fix: pak elvis nggak bisa
</commit_message>
<xml_diff>
--- a/jadwal.xlsx
+++ b/jadwal.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20402"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948D358F-8581-485B-A9EB-7F9678F99EEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0647E4A2-F353-4C0D-9367-8D7AB589A5D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="87">
   <si>
     <t>Tanggal</t>
   </si>
@@ -269,9 +269,6 @@
   </si>
   <si>
     <t>Ustadz Yuda</t>
-  </si>
-  <si>
-    <t>Ustadz Elvis Indra</t>
   </si>
   <si>
     <t>Ustadz Awan Karliawan</t>
@@ -730,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,7 +741,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -753,7 +750,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -967,9 +964,7 @@
       <c r="C15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>83</v>
-      </c>
+      <c r="D15" s="8"/>
       <c r="E15" s="10"/>
       <c r="F15" t="s">
         <v>72</v>
@@ -1148,7 +1143,7 @@
         <v>21</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E25" s="10" t="s">
         <v>74</v>
@@ -1165,9 +1160,11 @@
         <v>22</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E26" s="10"/>
+        <v>83</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">

</xml_diff>

<commit_message>
fix: tinggal ustadz miftah
</commit_message>
<xml_diff>
--- a/jadwal.xlsx
+++ b/jadwal.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20402"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0647E4A2-F353-4C0D-9367-8D7AB589A5D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19900DDA-744A-4816-8EFC-6132C87C9ED9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="87">
   <si>
     <t>Tanggal</t>
   </si>
@@ -727,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,7 +1179,9 @@
       <c r="D27" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="E27" s="10"/>
+      <c r="E27" s="10" t="s">
+        <v>74</v>
+      </c>
       <c r="F27" t="s">
         <v>70</v>
       </c>
@@ -1214,7 +1216,9 @@
       <c r="D29" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="E29" s="10"/>
+      <c r="E29" s="10" t="s">
+        <v>74</v>
+      </c>
       <c r="F29" t="s">
         <v>73</v>
       </c>
@@ -1249,7 +1253,9 @@
       <c r="D31" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="E31" s="10"/>
+      <c r="E31" s="10" t="s">
+        <v>74</v>
+      </c>
       <c r="F31" t="s">
         <v>69</v>
       </c>
@@ -1284,7 +1290,9 @@
       <c r="D33" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="E33" s="10"/>
+      <c r="E33" s="10" t="s">
+        <v>74</v>
+      </c>
       <c r="F33" t="s">
         <v>72</v>
       </c>

</xml_diff>

<commit_message>
fix: coba tawarkan ke ustadz wahidi
</commit_message>
<xml_diff>
--- a/jadwal.xlsx
+++ b/jadwal.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20402"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19900DDA-744A-4816-8EFC-6132C87C9ED9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15399DFB-B420-45AE-A33C-04072A80221A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="87">
   <si>
     <t>Tanggal</t>
   </si>
@@ -727,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,7 +880,9 @@
       <c r="D10" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="10"/>
+      <c r="E10" s="10" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -913,7 +915,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E12" s="10"/>
     </row>
@@ -964,7 +966,9 @@
       <c r="C15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="8"/>
+      <c r="D15" s="8" t="s">
+        <v>70</v>
+      </c>
       <c r="E15" s="10"/>
       <c r="F15" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
fix: ada kosong satu
</commit_message>
<xml_diff>
--- a/jadwal.xlsx
+++ b/jadwal.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20402"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15399DFB-B420-45AE-A33C-04072A80221A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{815CEB5C-5E07-4958-A67D-3DF6FA5B399D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="87">
   <si>
     <t>Tanggal</t>
   </si>
@@ -728,7 +728,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,9 +914,7 @@
       <c r="C12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>70</v>
-      </c>
+      <c r="D12" s="8"/>
       <c r="E12" s="10"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix: masih kosong satu
</commit_message>
<xml_diff>
--- a/jadwal.xlsx
+++ b/jadwal.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20402"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{815CEB5C-5E07-4958-A67D-3DF6FA5B399D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261D540C-66F1-4BDC-9B89-C531295F54F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="87">
   <si>
     <t>Tanggal</t>
   </si>
@@ -728,7 +728,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,7 +967,9 @@
       <c r="D15" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="10"/>
+      <c r="E15" s="10" t="s">
+        <v>74</v>
+      </c>
       <c r="F15" t="s">
         <v>72</v>
       </c>

</xml_diff>